<commit_message>
correção de melhor valor mutação d2
</commit_message>
<xml_diff>
--- a/Experimentos/teste_mutacao/Testes Mutação Total.xlsx
+++ b/Experimentos/teste_mutacao/Testes Mutação Total.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\ESCOLA\2ano\2semestre\INTELIGENCIA-ARTIFICIAL\projeto-IA\Experimentos\teste_mutacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7E7008-2911-4557-A113-BC3FE1454DA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE1CD4D-45A1-47CA-BAE1-F5F071A681D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="629" xr2:uid="{087E5C9E-DC88-4174-9BF2-C4B7AD4ED23E}"/>
+    <workbookView xWindow="-19320" yWindow="-5595" windowWidth="19440" windowHeight="15000" tabRatio="629" xr2:uid="{087E5C9E-DC88-4174-9BF2-C4B7AD4ED23E}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráficos" sheetId="11" r:id="rId1"/>
@@ -251,6 +251,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -269,32 +280,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -319,9 +304,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1720,64 +1720,64 @@
                 <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2195,7 +2195,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -2205,6 +2205,25 @@
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-A5EC-4E54-8AC4-CF6C1FD2389F}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-6A11-4922-8C9C-FE4E53BE411F}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -2291,64 +2310,64 @@
                 <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2843,64 +2862,64 @@
                 <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3400,64 +3419,64 @@
                 <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3957,64 +3976,64 @@
                 <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -5061,64 +5080,64 @@
                 <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -5613,64 +5632,64 @@
                 <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -6165,64 +6184,64 @@
                 <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.1</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0.2</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.3</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>0.4</c:v>
+                    <c:v>0,4</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>0.5</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -6640,7 +6659,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -23484,7 +23503,9 @@
   </sheetPr>
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="18" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23654,7 +23675,7 @@
       <c r="E2" s="5">
         <v>0.8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5">
@@ -23690,7 +23711,7 @@
       <c r="E3" s="8">
         <v>0.8</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="8">
         <v>0.2</v>
       </c>
@@ -23724,7 +23745,7 @@
       <c r="E4" s="5">
         <v>0.8</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="5">
         <v>0.3</v>
       </c>
@@ -23758,7 +23779,7 @@
       <c r="E5" s="8">
         <v>0.8</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="8">
         <v>0.4</v>
       </c>
@@ -23792,7 +23813,7 @@
       <c r="E6" s="5">
         <v>0.8</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
@@ -23826,7 +23847,7 @@
       <c r="E7" s="8">
         <v>0.8</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="8">
@@ -23862,7 +23883,7 @@
       <c r="E8" s="5">
         <v>0.8</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="5">
         <v>0.2</v>
       </c>
@@ -23896,7 +23917,7 @@
       <c r="E9" s="8">
         <v>0.8</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="8">
         <v>0.3</v>
       </c>
@@ -23930,7 +23951,7 @@
       <c r="E10" s="5">
         <v>0.8</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="5">
         <v>0.4</v>
       </c>
@@ -23964,7 +23985,7 @@
       <c r="E11" s="8">
         <v>0.8</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="8">
         <v>0.5</v>
       </c>
@@ -23998,7 +24019,7 @@
       <c r="E12" s="5">
         <v>0.8</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="5">
@@ -24034,7 +24055,7 @@
       <c r="E13" s="8">
         <v>0.8</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="8">
         <v>0.2</v>
       </c>
@@ -24068,7 +24089,7 @@
       <c r="E14" s="5">
         <v>0.8</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="5">
         <v>0.3</v>
       </c>
@@ -24102,7 +24123,7 @@
       <c r="E15" s="8">
         <v>0.8</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="8">
         <v>0.4</v>
       </c>
@@ -24136,7 +24157,7 @@
       <c r="E16" s="5">
         <v>0.8</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="5">
         <v>0.5</v>
       </c>
@@ -24170,7 +24191,7 @@
       <c r="E17" s="8">
         <v>0.8</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8">
@@ -24206,7 +24227,7 @@
       <c r="E18" s="5">
         <v>0.8</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="5">
         <v>0.2</v>
       </c>
@@ -24240,7 +24261,7 @@
       <c r="E19" s="8">
         <v>0.8</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="8">
         <v>0.3</v>
       </c>
@@ -24274,7 +24295,7 @@
       <c r="E20" s="5">
         <v>0.8</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="5">
         <v>0.4</v>
       </c>
@@ -24308,7 +24329,7 @@
       <c r="E21" s="11">
         <v>0.8</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="11">
         <v>0.5</v>
       </c>
@@ -24407,14 +24428,14 @@
       <c r="E2" s="5">
         <v>0.8</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="39" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5">
         <v>0.1</v>
       </c>
       <c r="H2" s="5"/>
-      <c r="I2" s="42">
+      <c r="I2" s="22">
         <v>3594.2</v>
       </c>
       <c r="J2" s="5">
@@ -24443,12 +24464,12 @@
       <c r="E3" s="8">
         <v>0.8</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="8">
         <v>0.2</v>
       </c>
       <c r="H3" s="8"/>
-      <c r="I3" s="43">
+      <c r="I3" s="23">
         <v>3576.86666666666</v>
       </c>
       <c r="J3" s="8">
@@ -24477,12 +24498,12 @@
       <c r="E4" s="5">
         <v>0.8</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="5">
         <v>0.3</v>
       </c>
       <c r="H4" s="5"/>
-      <c r="I4" s="42">
+      <c r="I4" s="22">
         <v>3542.7333333333299</v>
       </c>
       <c r="J4" s="5">
@@ -24511,12 +24532,12 @@
       <c r="E5" s="8">
         <v>0.8</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="40"/>
       <c r="G5" s="8">
         <v>0.4</v>
       </c>
       <c r="H5" s="8"/>
-      <c r="I5" s="43">
+      <c r="I5" s="23">
         <v>3524.8</v>
       </c>
       <c r="J5" s="8">
@@ -24545,12 +24566,12 @@
       <c r="E6" s="5">
         <v>0.8</v>
       </c>
-      <c r="F6" s="22"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="42">
+      <c r="I6" s="22">
         <v>3496.9333333333302</v>
       </c>
       <c r="J6" s="5">
@@ -24579,14 +24600,14 @@
       <c r="E7" s="8">
         <v>0.8</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="42" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="8">
         <v>0.1</v>
       </c>
       <c r="H7" s="8"/>
-      <c r="I7" s="43">
+      <c r="I7" s="23">
         <v>3595.5333333333301</v>
       </c>
       <c r="J7" s="8">
@@ -24615,12 +24636,12 @@
       <c r="E8" s="5">
         <v>0.8</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="5">
         <v>0.2</v>
       </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="42">
+      <c r="I8" s="22">
         <v>3520.3333333333298</v>
       </c>
       <c r="J8" s="5">
@@ -24649,12 +24670,12 @@
       <c r="E9" s="8">
         <v>0.8</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="8">
         <v>0.3</v>
       </c>
       <c r="H9" s="8"/>
-      <c r="I9" s="43">
+      <c r="I9" s="23">
         <v>3511.6666666666601</v>
       </c>
       <c r="J9" s="8">
@@ -24683,12 +24704,12 @@
       <c r="E10" s="5">
         <v>0.8</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="5">
         <v>0.4</v>
       </c>
       <c r="H10" s="5"/>
-      <c r="I10" s="42">
+      <c r="I10" s="22">
         <v>3463.13333333333</v>
       </c>
       <c r="J10" s="5">
@@ -24717,12 +24738,12 @@
       <c r="E11" s="8">
         <v>0.8</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="8">
         <v>0.5</v>
       </c>
       <c r="H11" s="8"/>
-      <c r="I11" s="43">
+      <c r="I11" s="23">
         <v>3391.7333333333299</v>
       </c>
       <c r="J11" s="8">
@@ -24751,14 +24772,14 @@
       <c r="E12" s="5">
         <v>0.8</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="39" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="5">
         <v>0.1</v>
       </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="42">
+      <c r="I12" s="22">
         <v>3575.7333333333299</v>
       </c>
       <c r="J12" s="5">
@@ -24787,12 +24808,12 @@
       <c r="E13" s="8">
         <v>0.8</v>
       </c>
-      <c r="F13" s="21"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="8">
         <v>0.2</v>
       </c>
       <c r="H13" s="8"/>
-      <c r="I13" s="43">
+      <c r="I13" s="23">
         <v>3516.4</v>
       </c>
       <c r="J13" s="8">
@@ -24821,12 +24842,12 @@
       <c r="E14" s="5">
         <v>0.8</v>
       </c>
-      <c r="F14" s="21"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="5">
         <v>0.3</v>
       </c>
       <c r="H14" s="5"/>
-      <c r="I14" s="42">
+      <c r="I14" s="22">
         <v>3489.13333333333</v>
       </c>
       <c r="J14" s="5">
@@ -24855,12 +24876,12 @@
       <c r="E15" s="8">
         <v>0.8</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="40"/>
       <c r="G15" s="8">
         <v>0.4</v>
       </c>
       <c r="H15" s="8"/>
-      <c r="I15" s="43">
+      <c r="I15" s="23">
         <v>3452.6666666666601</v>
       </c>
       <c r="J15" s="8">
@@ -24889,12 +24910,12 @@
       <c r="E16" s="5">
         <v>0.8</v>
       </c>
-      <c r="F16" s="22"/>
+      <c r="F16" s="41"/>
       <c r="G16" s="5">
         <v>0.5</v>
       </c>
       <c r="H16" s="5"/>
-      <c r="I16" s="42">
+      <c r="I16" s="22">
         <v>3416.3333333333298</v>
       </c>
       <c r="J16" s="5">
@@ -24923,14 +24944,14 @@
       <c r="E17" s="8">
         <v>0.8</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="42" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8">
         <v>0.1</v>
       </c>
       <c r="H17" s="8"/>
-      <c r="I17" s="43">
+      <c r="I17" s="23">
         <v>2837.6</v>
       </c>
       <c r="J17" s="8">
@@ -24959,12 +24980,12 @@
       <c r="E18" s="5">
         <v>0.8</v>
       </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="43"/>
       <c r="G18" s="5">
         <v>0.2</v>
       </c>
       <c r="H18" s="5"/>
-      <c r="I18" s="42">
+      <c r="I18" s="22">
         <v>2790.9333333333302</v>
       </c>
       <c r="J18" s="5">
@@ -24993,12 +25014,12 @@
       <c r="E19" s="8">
         <v>0.8</v>
       </c>
-      <c r="F19" s="24"/>
+      <c r="F19" s="43"/>
       <c r="G19" s="8">
         <v>0.3</v>
       </c>
       <c r="H19" s="8"/>
-      <c r="I19" s="43">
+      <c r="I19" s="23">
         <v>2787.7333333333299</v>
       </c>
       <c r="J19" s="8">
@@ -25027,12 +25048,12 @@
       <c r="E20" s="5">
         <v>0.8</v>
       </c>
-      <c r="F20" s="24"/>
+      <c r="F20" s="43"/>
       <c r="G20" s="5">
         <v>0.4</v>
       </c>
       <c r="H20" s="5"/>
-      <c r="I20" s="42">
+      <c r="I20" s="22">
         <v>2778.86666666666</v>
       </c>
       <c r="J20" s="5">
@@ -25061,12 +25082,12 @@
       <c r="E21" s="11">
         <v>0.8</v>
       </c>
-      <c r="F21" s="25"/>
+      <c r="F21" s="44"/>
       <c r="G21" s="11">
         <v>0.5</v>
       </c>
       <c r="H21" s="11"/>
-      <c r="I21" s="44">
+      <c r="I21" s="24">
         <v>2759.86666666666</v>
       </c>
       <c r="J21" s="11">
@@ -25170,7 +25191,7 @@
       <c r="E2" s="5">
         <v>0.7</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5">
@@ -25206,7 +25227,7 @@
       <c r="E3" s="8">
         <v>0.7</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="8">
         <v>0.2</v>
       </c>
@@ -25240,7 +25261,7 @@
       <c r="E4" s="5">
         <v>0.7</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="5">
         <v>0.3</v>
       </c>
@@ -25274,7 +25295,7 @@
       <c r="E5" s="8">
         <v>0.7</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="8">
         <v>0.4</v>
       </c>
@@ -25308,7 +25329,7 @@
       <c r="E6" s="5">
         <v>0.7</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
@@ -25342,7 +25363,7 @@
       <c r="E7" s="8">
         <v>0.7</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="8">
@@ -25378,7 +25399,7 @@
       <c r="E8" s="5">
         <v>0.7</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="5">
         <v>0.2</v>
       </c>
@@ -25412,7 +25433,7 @@
       <c r="E9" s="8">
         <v>0.7</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="8">
         <v>0.3</v>
       </c>
@@ -25446,7 +25467,7 @@
       <c r="E10" s="5">
         <v>0.7</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="5">
         <v>0.4</v>
       </c>
@@ -25480,7 +25501,7 @@
       <c r="E11" s="8">
         <v>0.7</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="8">
         <v>0.5</v>
       </c>
@@ -25514,7 +25535,7 @@
       <c r="E12" s="5">
         <v>0.7</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="5">
@@ -25550,7 +25571,7 @@
       <c r="E13" s="8">
         <v>0.7</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="8">
         <v>0.2</v>
       </c>
@@ -25584,7 +25605,7 @@
       <c r="E14" s="5">
         <v>0.7</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="5">
         <v>0.3</v>
       </c>
@@ -25618,7 +25639,7 @@
       <c r="E15" s="8">
         <v>0.7</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="8">
         <v>0.4</v>
       </c>
@@ -25652,7 +25673,7 @@
       <c r="E16" s="5">
         <v>0.7</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="5">
         <v>0.5</v>
       </c>
@@ -25686,7 +25707,7 @@
       <c r="E17" s="8">
         <v>0.7</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8">
@@ -25722,7 +25743,7 @@
       <c r="E18" s="5">
         <v>0.7</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="13">
         <v>0.2</v>
       </c>
@@ -25756,7 +25777,7 @@
       <c r="E19" s="8">
         <v>0.7</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="8">
         <v>0.3</v>
       </c>
@@ -25790,7 +25811,7 @@
       <c r="E20" s="5">
         <v>0.7</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="5">
         <v>0.4</v>
       </c>
@@ -25824,7 +25845,7 @@
       <c r="E21" s="11">
         <v>0.7</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="11">
         <v>0.5</v>
       </c>
@@ -25860,8 +25881,8 @@
   <sheetPr codeName="Folha3"/>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25923,7 +25944,7 @@
       <c r="E2" s="5">
         <v>0.8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5">
@@ -25959,7 +25980,7 @@
       <c r="E3" s="8">
         <v>0.8</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="8">
         <v>0.2</v>
       </c>
@@ -25993,7 +26014,7 @@
       <c r="E4" s="5">
         <v>0.8</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="5">
         <v>0.3</v>
       </c>
@@ -26027,7 +26048,7 @@
       <c r="E5" s="8">
         <v>0.8</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="8">
         <v>0.4</v>
       </c>
@@ -26061,7 +26082,7 @@
       <c r="E6" s="5">
         <v>0.8</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
@@ -26095,7 +26116,7 @@
       <c r="E7" s="8">
         <v>0.8</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="8">
@@ -26131,7 +26152,7 @@
       <c r="E8" s="5">
         <v>0.8</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="5">
         <v>0.2</v>
       </c>
@@ -26165,7 +26186,7 @@
       <c r="E9" s="8">
         <v>0.8</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="8">
         <v>0.3</v>
       </c>
@@ -26199,7 +26220,7 @@
       <c r="E10" s="5">
         <v>0.8</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="5">
         <v>0.4</v>
       </c>
@@ -26233,7 +26254,7 @@
       <c r="E11" s="8">
         <v>0.8</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="8">
         <v>0.5</v>
       </c>
@@ -26267,7 +26288,7 @@
       <c r="E12" s="5">
         <v>0.8</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="5">
@@ -26303,7 +26324,7 @@
       <c r="E13" s="8">
         <v>0.8</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="8">
         <v>0.2</v>
       </c>
@@ -26337,7 +26358,7 @@
       <c r="E14" s="5">
         <v>0.8</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="5">
         <v>0.3</v>
       </c>
@@ -26371,7 +26392,7 @@
       <c r="E15" s="8">
         <v>0.8</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="8">
         <v>0.4</v>
       </c>
@@ -26405,7 +26426,7 @@
       <c r="E16" s="5">
         <v>0.8</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="5">
         <v>0.5</v>
       </c>
@@ -26439,7 +26460,7 @@
       <c r="E17" s="8">
         <v>0.8</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8">
@@ -26475,7 +26496,7 @@
       <c r="E18" s="5">
         <v>0.8</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="5">
         <v>0.2</v>
       </c>
@@ -26509,7 +26530,7 @@
       <c r="E19" s="8">
         <v>0.8</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="8">
         <v>0.3</v>
       </c>
@@ -26543,7 +26564,7 @@
       <c r="E20" s="5">
         <v>0.8</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="5">
         <v>0.4</v>
       </c>
@@ -26577,7 +26598,7 @@
       <c r="E21" s="11">
         <v>0.8</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="11">
         <v>0.5</v>
       </c>
@@ -26675,7 +26696,7 @@
       <c r="E2" s="5">
         <v>0.8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5">
@@ -26711,7 +26732,7 @@
       <c r="E3" s="8">
         <v>0.8</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="8">
         <v>0.2</v>
       </c>
@@ -26745,7 +26766,7 @@
       <c r="E4" s="5">
         <v>0.8</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="5">
         <v>0.3</v>
       </c>
@@ -26779,7 +26800,7 @@
       <c r="E5" s="8">
         <v>0.8</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="8">
         <v>0.4</v>
       </c>
@@ -26813,7 +26834,7 @@
       <c r="E6" s="5">
         <v>0.8</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
@@ -26847,7 +26868,7 @@
       <c r="E7" s="8">
         <v>0.8</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="8">
@@ -26883,7 +26904,7 @@
       <c r="E8" s="5">
         <v>0.8</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="5">
         <v>0.2</v>
       </c>
@@ -26917,7 +26938,7 @@
       <c r="E9" s="8">
         <v>0.8</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="8">
         <v>0.3</v>
       </c>
@@ -26951,7 +26972,7 @@
       <c r="E10" s="5">
         <v>0.8</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="5">
         <v>0.4</v>
       </c>
@@ -26985,7 +27006,7 @@
       <c r="E11" s="8">
         <v>0.8</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="8">
         <v>0.5</v>
       </c>
@@ -27019,7 +27040,7 @@
       <c r="E12" s="5">
         <v>0.8</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="5">
@@ -27055,7 +27076,7 @@
       <c r="E13" s="8">
         <v>0.8</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="8">
         <v>0.2</v>
       </c>
@@ -27089,7 +27110,7 @@
       <c r="E14" s="5">
         <v>0.8</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="5">
         <v>0.3</v>
       </c>
@@ -27123,7 +27144,7 @@
       <c r="E15" s="8">
         <v>0.8</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="8">
         <v>0.4</v>
       </c>
@@ -27157,7 +27178,7 @@
       <c r="E16" s="5">
         <v>0.8</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="5">
         <v>0.5</v>
       </c>
@@ -27191,7 +27212,7 @@
       <c r="E17" s="8">
         <v>0.8</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8">
@@ -27227,7 +27248,7 @@
       <c r="E18" s="5">
         <v>0.8</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="5">
         <v>0.2</v>
       </c>
@@ -27261,7 +27282,7 @@
       <c r="E19" s="8">
         <v>0.8</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="8">
         <v>0.3</v>
       </c>
@@ -27295,7 +27316,7 @@
       <c r="E20" s="5">
         <v>0.8</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="5">
         <v>0.4</v>
       </c>
@@ -27329,7 +27350,7 @@
       <c r="E21" s="11">
         <v>0.8</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="11">
         <v>0.5</v>
       </c>
@@ -27427,7 +27448,7 @@
       <c r="E2" s="5">
         <v>0.8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5">
@@ -27463,7 +27484,7 @@
       <c r="E3" s="8">
         <v>0.8</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="8">
         <v>0.2</v>
       </c>
@@ -27497,7 +27518,7 @@
       <c r="E4" s="5">
         <v>0.8</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="5">
         <v>0.3</v>
       </c>
@@ -27531,7 +27552,7 @@
       <c r="E5" s="8">
         <v>0.8</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="8">
         <v>0.4</v>
       </c>
@@ -27565,7 +27586,7 @@
       <c r="E6" s="5">
         <v>0.8</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
@@ -27599,7 +27620,7 @@
       <c r="E7" s="8">
         <v>0.8</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="8">
@@ -27635,7 +27656,7 @@
       <c r="E8" s="5">
         <v>0.8</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="5">
         <v>0.2</v>
       </c>
@@ -27669,7 +27690,7 @@
       <c r="E9" s="8">
         <v>0.8</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="8">
         <v>0.3</v>
       </c>
@@ -27703,7 +27724,7 @@
       <c r="E10" s="5">
         <v>0.8</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="5">
         <v>0.4</v>
       </c>
@@ -27737,7 +27758,7 @@
       <c r="E11" s="8">
         <v>0.8</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="8">
         <v>0.5</v>
       </c>
@@ -27771,7 +27792,7 @@
       <c r="E12" s="5">
         <v>0.8</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="5">
@@ -27807,7 +27828,7 @@
       <c r="E13" s="8">
         <v>0.8</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="8">
         <v>0.2</v>
       </c>
@@ -27841,7 +27862,7 @@
       <c r="E14" s="5">
         <v>0.8</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="5">
         <v>0.3</v>
       </c>
@@ -27875,7 +27896,7 @@
       <c r="E15" s="8">
         <v>0.8</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="8">
         <v>0.4</v>
       </c>
@@ -27909,7 +27930,7 @@
       <c r="E16" s="5">
         <v>0.8</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="5">
         <v>0.5</v>
       </c>
@@ -27943,7 +27964,7 @@
       <c r="E17" s="8">
         <v>0.8</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8">
@@ -27979,7 +28000,7 @@
       <c r="E18" s="5">
         <v>0.8</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="5">
         <v>0.2</v>
       </c>
@@ -28013,7 +28034,7 @@
       <c r="E19" s="8">
         <v>0.8</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="8">
         <v>0.3</v>
       </c>
@@ -28047,7 +28068,7 @@
       <c r="E20" s="5">
         <v>0.8</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="5">
         <v>0.4</v>
       </c>
@@ -28081,7 +28102,7 @@
       <c r="E21" s="11">
         <v>0.8</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="11">
         <v>0.5</v>
       </c>
@@ -28175,7 +28196,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="14">
         <v>200</v>
       </c>
       <c r="B2" s="13">
@@ -28190,7 +28211,7 @@
       <c r="E2" s="13">
         <v>0.8</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="31" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="13">
@@ -28206,46 +28227,46 @@
       <c r="K2" s="13">
         <v>3493.48</v>
       </c>
-      <c r="L2" s="27">
+      <c r="L2" s="15">
         <v>6562.94</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="28">
+      <c r="A3" s="16">
         <v>200</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="17">
         <v>3500</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="17">
         <v>0.8</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="29">
+      <c r="F3" s="32"/>
+      <c r="G3" s="17">
         <v>0.2</v>
       </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17">
         <v>219.92</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="17">
         <v>32.082294182305603</v>
       </c>
-      <c r="K3" s="29">
+      <c r="K3" s="17">
         <v>5798.76</v>
       </c>
-      <c r="L3" s="30">
+      <c r="L3" s="18">
         <v>7009.62</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
+      <c r="A4" s="14">
         <v>200</v>
       </c>
       <c r="B4" s="13">
@@ -28260,7 +28281,7 @@
       <c r="E4" s="13">
         <v>0.8</v>
       </c>
-      <c r="F4" s="35"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="13">
         <v>0.3</v>
       </c>
@@ -28274,46 +28295,46 @@
       <c r="K4" s="13">
         <v>3560.78</v>
       </c>
-      <c r="L4" s="27">
+      <c r="L4" s="15">
         <v>8213.0400000000009</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="A5" s="16">
         <v>200</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="17">
         <v>3500</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="17">
         <v>0.8</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="29">
+      <c r="F5" s="32"/>
+      <c r="G5" s="17">
         <v>0.4</v>
       </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29">
+      <c r="H5" s="17"/>
+      <c r="I5" s="17">
         <v>402.32</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="17">
         <v>6.4169774816497496</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="17">
         <v>3867.3</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="18">
         <v>8245.34</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="14">
         <v>200</v>
       </c>
       <c r="B6" s="13">
@@ -28328,7 +28349,7 @@
       <c r="E6" s="13">
         <v>0.8</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="13">
         <v>0.5</v>
       </c>
@@ -28342,48 +28363,48 @@
       <c r="K6" s="13">
         <v>3949.36</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L6" s="15">
         <v>8221.3799999999992</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="A7" s="16">
         <v>200</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="17">
         <v>3500</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="17">
         <v>0.8</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="17">
         <v>0.1</v>
       </c>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29">
+      <c r="H7" s="17"/>
+      <c r="I7" s="17">
         <v>228.8</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="17">
         <v>15.0784614599766</v>
       </c>
-      <c r="K7" s="29">
+      <c r="K7" s="17">
         <v>4614.38</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="18">
         <v>6535.26</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="A8" s="14">
         <v>200</v>
       </c>
       <c r="B8" s="13">
@@ -28398,7 +28419,7 @@
       <c r="E8" s="13">
         <v>0.8</v>
       </c>
-      <c r="F8" s="38"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="13">
         <v>0.2</v>
       </c>
@@ -28412,46 +28433,46 @@
       <c r="K8" s="13">
         <v>5850.64</v>
       </c>
-      <c r="L8" s="27">
+      <c r="L8" s="15">
         <v>7639.26</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="16">
         <v>200</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="17">
         <v>3500</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="17">
         <v>0.8</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="29">
+      <c r="F9" s="35"/>
+      <c r="G9" s="17">
         <v>0.3</v>
       </c>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29">
+      <c r="H9" s="17"/>
+      <c r="I9" s="17">
         <v>407.36</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="17">
         <v>7.47732572515066</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9" s="17">
         <v>4019.5</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="18">
         <v>8188.14</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="26">
+      <c r="A10" s="14">
         <v>200</v>
       </c>
       <c r="B10" s="13">
@@ -28466,7 +28487,7 @@
       <c r="E10" s="13">
         <v>0.8</v>
       </c>
-      <c r="F10" s="38"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="13">
         <v>0.4</v>
       </c>
@@ -28480,46 +28501,46 @@
       <c r="K10" s="13">
         <v>3268.5</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="15">
         <v>8197.42</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="A11" s="16">
         <v>200</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="17">
         <v>3500</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="17">
         <v>0.8</v>
       </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="29">
+      <c r="F11" s="36"/>
+      <c r="G11" s="17">
         <v>0.5</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29">
+      <c r="H11" s="17"/>
+      <c r="I11" s="17">
         <v>412.2</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="17">
         <v>8.1018516402116401</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11" s="17">
         <v>4116.9399999999996</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="18">
         <v>8209.2199999999993</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="26">
+      <c r="A12" s="14">
         <v>200</v>
       </c>
       <c r="B12" s="13">
@@ -28534,7 +28555,7 @@
       <c r="E12" s="13">
         <v>0.8</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="31" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="13">
@@ -28550,46 +28571,46 @@
       <c r="K12" s="13">
         <v>4838.24</v>
       </c>
-      <c r="L12" s="27">
+      <c r="L12" s="15">
         <v>6636.94</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="A13" s="16">
         <v>200</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="17">
         <v>3500</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="17">
         <v>0.8</v>
       </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="29">
+      <c r="F13" s="32"/>
+      <c r="G13" s="17">
         <v>0.2</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29">
+      <c r="H13" s="17"/>
+      <c r="I13" s="17">
         <v>214.84</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="17">
         <v>24.5734490863614</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="17">
         <v>6242.12</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="18">
         <v>7204.62</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="26">
+      <c r="A14" s="14">
         <v>200</v>
       </c>
       <c r="B14" s="13">
@@ -28604,7 +28625,7 @@
       <c r="E14" s="13">
         <v>0.8</v>
       </c>
-      <c r="F14" s="35"/>
+      <c r="F14" s="32"/>
       <c r="G14" s="13">
         <v>0.3</v>
       </c>
@@ -28618,46 +28639,46 @@
       <c r="K14" s="13">
         <v>4197.78</v>
       </c>
-      <c r="L14" s="27">
+      <c r="L14" s="15">
         <v>8325.36</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+      <c r="A15" s="16">
         <v>200</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="17">
         <v>3500</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="17">
         <v>0.8</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="29">
+      <c r="F15" s="32"/>
+      <c r="G15" s="17">
         <v>0.4</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29">
+      <c r="H15" s="17"/>
+      <c r="I15" s="17">
         <v>410.36</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="17">
         <v>6.7845707307094898</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="17">
         <v>4162</v>
       </c>
-      <c r="L15" s="30">
+      <c r="L15" s="18">
         <v>8311.52</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="26">
+      <c r="A16" s="14">
         <v>200</v>
       </c>
       <c r="B16" s="13">
@@ -28672,7 +28693,7 @@
       <c r="E16" s="13">
         <v>0.8</v>
       </c>
-      <c r="F16" s="36"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="13">
         <v>0.5</v>
       </c>
@@ -28686,48 +28707,48 @@
       <c r="K16" s="13">
         <v>3825.34</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="15">
         <v>8253.08</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="16">
         <v>200</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="17">
         <v>3500</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="17">
         <v>0.8</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="17">
         <v>0.1</v>
       </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29">
+      <c r="H17" s="17"/>
+      <c r="I17" s="17">
         <v>185.84</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="17">
         <v>12.301804745646001</v>
       </c>
-      <c r="K17" s="29">
+      <c r="K17" s="17">
         <v>3997.3</v>
       </c>
-      <c r="L17" s="30">
+      <c r="L17" s="18">
         <v>6398.04</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+      <c r="A18" s="14">
         <v>200</v>
       </c>
       <c r="B18" s="13">
@@ -28742,7 +28763,7 @@
       <c r="E18" s="13">
         <v>0.8</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="13">
         <v>0.2</v>
       </c>
@@ -28756,46 +28777,46 @@
       <c r="K18" s="13">
         <v>4093.8</v>
       </c>
-      <c r="L18" s="27">
+      <c r="L18" s="15">
         <v>6464.18</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="28">
+      <c r="A19" s="16">
         <v>200</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="17">
         <v>3500</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="17">
         <v>0.8</v>
       </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="29">
+      <c r="F19" s="35"/>
+      <c r="G19" s="17">
         <v>0.3</v>
       </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29">
+      <c r="H19" s="17"/>
+      <c r="I19" s="17">
         <v>171.04</v>
       </c>
-      <c r="J19" s="29">
+      <c r="J19" s="17">
         <v>13.8231110825313</v>
       </c>
-      <c r="K19" s="29">
+      <c r="K19" s="17">
         <v>4512.9399999999996</v>
       </c>
-      <c r="L19" s="30">
+      <c r="L19" s="18">
         <v>6560.32</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="26">
+      <c r="A20" s="14">
         <v>200</v>
       </c>
       <c r="B20" s="13">
@@ -28810,7 +28831,7 @@
       <c r="E20" s="13">
         <v>0.8</v>
       </c>
-      <c r="F20" s="38"/>
+      <c r="F20" s="35"/>
       <c r="G20" s="13">
         <v>0.4</v>
       </c>
@@ -28824,41 +28845,41 @@
       <c r="K20" s="13">
         <v>5466.56</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L20" s="15">
         <v>6953.16</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="31">
+      <c r="A21" s="19">
         <v>200</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="20">
         <v>3500</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="20">
         <v>0.8</v>
       </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="32">
+      <c r="F21" s="36"/>
+      <c r="G21" s="20">
         <v>0.5</v>
       </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32">
+      <c r="H21" s="20"/>
+      <c r="I21" s="20">
         <v>297.83999999999997</v>
       </c>
-      <c r="J21" s="32">
+      <c r="J21" s="20">
         <v>16.979234376143101</v>
       </c>
-      <c r="K21" s="32">
+      <c r="K21" s="20">
         <v>5315.04</v>
       </c>
-      <c r="L21" s="33">
+      <c r="L21" s="21">
         <v>7865.12</v>
       </c>
     </row>
@@ -28942,7 +28963,7 @@
       <c r="E2" s="5">
         <v>0.8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5">
@@ -28978,7 +28999,7 @@
       <c r="E3" s="8">
         <v>0.8</v>
       </c>
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="8">
         <v>0.2</v>
       </c>
@@ -29012,7 +29033,7 @@
       <c r="E4" s="5">
         <v>0.8</v>
       </c>
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="5">
         <v>0.3</v>
       </c>
@@ -29046,7 +29067,7 @@
       <c r="E5" s="8">
         <v>0.8</v>
       </c>
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="8">
         <v>0.4</v>
       </c>
@@ -29080,7 +29101,7 @@
       <c r="E6" s="5">
         <v>0.8</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
@@ -29114,7 +29135,7 @@
       <c r="E7" s="8">
         <v>0.8</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="8">
@@ -29150,7 +29171,7 @@
       <c r="E8" s="5">
         <v>0.8</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="5">
         <v>0.2</v>
       </c>
@@ -29184,7 +29205,7 @@
       <c r="E9" s="8">
         <v>0.8</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="8">
         <v>0.3</v>
       </c>
@@ -29218,7 +29239,7 @@
       <c r="E10" s="5">
         <v>0.8</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="5">
         <v>0.4</v>
       </c>
@@ -29252,7 +29273,7 @@
       <c r="E11" s="8">
         <v>0.8</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="8">
         <v>0.5</v>
       </c>
@@ -29286,7 +29307,7 @@
       <c r="E12" s="5">
         <v>0.8</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="5">
@@ -29322,7 +29343,7 @@
       <c r="E13" s="8">
         <v>0.8</v>
       </c>
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="8">
         <v>0.2</v>
       </c>
@@ -29356,7 +29377,7 @@
       <c r="E14" s="5">
         <v>0.8</v>
       </c>
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
       <c r="G14" s="5">
         <v>0.3</v>
       </c>
@@ -29390,7 +29411,7 @@
       <c r="E15" s="8">
         <v>0.8</v>
       </c>
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="8">
         <v>0.4</v>
       </c>
@@ -29424,7 +29445,7 @@
       <c r="E16" s="5">
         <v>0.8</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="5">
         <v>0.5</v>
       </c>
@@ -29458,7 +29479,7 @@
       <c r="E17" s="8">
         <v>0.8</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8">
@@ -29494,7 +29515,7 @@
       <c r="E18" s="5">
         <v>0.8</v>
       </c>
-      <c r="F18" s="41"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="5">
         <v>0.2</v>
       </c>
@@ -29528,7 +29549,7 @@
       <c r="E19" s="8">
         <v>0.8</v>
       </c>
-      <c r="F19" s="41"/>
+      <c r="F19" s="38"/>
       <c r="G19" s="8">
         <v>0.3</v>
       </c>
@@ -29562,7 +29583,7 @@
       <c r="E20" s="5">
         <v>0.8</v>
       </c>
-      <c r="F20" s="41"/>
+      <c r="F20" s="38"/>
       <c r="G20" s="5">
         <v>0.4</v>
       </c>
@@ -29596,7 +29617,7 @@
       <c r="E21" s="11">
         <v>0.8</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="11">
         <v>0.5</v>
       </c>
@@ -29694,7 +29715,7 @@
       <c r="E2" s="5">
         <v>0.8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5">
@@ -29730,7 +29751,7 @@
       <c r="E3" s="8">
         <v>0.8</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="8">
         <v>0.2</v>
       </c>
@@ -29764,7 +29785,7 @@
       <c r="E4" s="5">
         <v>0.8</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="5">
         <v>0.3</v>
       </c>
@@ -29798,7 +29819,7 @@
       <c r="E5" s="8">
         <v>0.8</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="8">
         <v>0.4</v>
       </c>
@@ -29832,7 +29853,7 @@
       <c r="E6" s="5">
         <v>0.8</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
@@ -29866,7 +29887,7 @@
       <c r="E7" s="8">
         <v>0.8</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="8">
@@ -29902,7 +29923,7 @@
       <c r="E8" s="5">
         <v>0.8</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="5">
         <v>0.2</v>
       </c>
@@ -29936,7 +29957,7 @@
       <c r="E9" s="8">
         <v>0.8</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="8">
         <v>0.3</v>
       </c>
@@ -29970,7 +29991,7 @@
       <c r="E10" s="5">
         <v>0.8</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="5">
         <v>0.4</v>
       </c>
@@ -30004,7 +30025,7 @@
       <c r="E11" s="8">
         <v>0.8</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="8">
         <v>0.5</v>
       </c>
@@ -30038,7 +30059,7 @@
       <c r="E12" s="5">
         <v>0.8</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="5">
@@ -30074,7 +30095,7 @@
       <c r="E13" s="8">
         <v>0.8</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="8">
         <v>0.2</v>
       </c>
@@ -30108,7 +30129,7 @@
       <c r="E14" s="5">
         <v>0.8</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="5">
         <v>0.3</v>
       </c>
@@ -30142,7 +30163,7 @@
       <c r="E15" s="8">
         <v>0.8</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="8">
         <v>0.4</v>
       </c>
@@ -30176,7 +30197,7 @@
       <c r="E16" s="5">
         <v>0.8</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="5">
         <v>0.5</v>
       </c>
@@ -30210,7 +30231,7 @@
       <c r="E17" s="8">
         <v>0.8</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8">
@@ -30246,7 +30267,7 @@
       <c r="E18" s="5">
         <v>0.8</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="5">
         <v>0.2</v>
       </c>
@@ -30280,7 +30301,7 @@
       <c r="E19" s="8">
         <v>0.8</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="8">
         <v>0.3</v>
       </c>
@@ -30314,7 +30335,7 @@
       <c r="E20" s="5">
         <v>0.8</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="5">
         <v>0.4</v>
       </c>
@@ -30348,7 +30369,7 @@
       <c r="E21" s="11">
         <v>0.8</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="11">
         <v>0.5</v>
       </c>
@@ -30446,7 +30467,7 @@
       <c r="E2" s="5">
         <v>0.7</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="5">
@@ -30482,7 +30503,7 @@
       <c r="E3" s="8">
         <v>0.7</v>
       </c>
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="8">
         <v>0.2</v>
       </c>
@@ -30516,7 +30537,7 @@
       <c r="E4" s="5">
         <v>0.7</v>
       </c>
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="5">
         <v>0.3</v>
       </c>
@@ -30550,7 +30571,7 @@
       <c r="E5" s="8">
         <v>0.7</v>
       </c>
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="8">
         <v>0.4</v>
       </c>
@@ -30584,7 +30605,7 @@
       <c r="E6" s="5">
         <v>0.7</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5">
         <v>0.5</v>
       </c>
@@ -30618,7 +30639,7 @@
       <c r="E7" s="8">
         <v>0.7</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="8">
@@ -30654,7 +30675,7 @@
       <c r="E8" s="5">
         <v>0.7</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="38"/>
       <c r="G8" s="5">
         <v>0.2</v>
       </c>
@@ -30688,7 +30709,7 @@
       <c r="E9" s="8">
         <v>0.7</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="8">
         <v>0.3</v>
       </c>
@@ -30722,7 +30743,7 @@
       <c r="E10" s="5">
         <v>0.7</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="5">
         <v>0.4</v>
       </c>
@@ -30756,7 +30777,7 @@
       <c r="E11" s="8">
         <v>0.7</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="8">
         <v>0.5</v>
       </c>
@@ -30790,7 +30811,7 @@
       <c r="E12" s="5">
         <v>0.7</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="5">
@@ -30826,7 +30847,7 @@
       <c r="E13" s="8">
         <v>0.7</v>
       </c>
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="8">
         <v>0.2</v>
       </c>
@@ -30860,7 +30881,7 @@
       <c r="E14" s="5">
         <v>0.7</v>
       </c>
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
       <c r="G14" s="5">
         <v>0.3</v>
       </c>
@@ -30894,7 +30915,7 @@
       <c r="E15" s="8">
         <v>0.7</v>
       </c>
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="8">
         <v>0.4</v>
       </c>
@@ -30928,7 +30949,7 @@
       <c r="E16" s="5">
         <v>0.7</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="5">
         <v>0.5</v>
       </c>
@@ -30962,7 +30983,7 @@
       <c r="E17" s="8">
         <v>0.7</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8">
@@ -30998,7 +31019,7 @@
       <c r="E18" s="5">
         <v>0.7</v>
       </c>
-      <c r="F18" s="41"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="5">
         <v>0.2</v>
       </c>
@@ -31032,7 +31053,7 @@
       <c r="E19" s="8">
         <v>0.7</v>
       </c>
-      <c r="F19" s="41"/>
+      <c r="F19" s="38"/>
       <c r="G19" s="8">
         <v>0.3</v>
       </c>
@@ -31066,7 +31087,7 @@
       <c r="E20" s="5">
         <v>0.7</v>
       </c>
-      <c r="F20" s="41"/>
+      <c r="F20" s="38"/>
       <c r="G20" s="5">
         <v>0.4</v>
       </c>
@@ -31100,7 +31121,7 @@
       <c r="E21" s="11">
         <v>0.7</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="11">
         <v>0.5</v>
       </c>

</xml_diff>